<commit_message>
Update Dataset for SWOT Analysis
</commit_message>
<xml_diff>
--- a/SWOT_Analysis/SWOT Analysis sample data.xlsx
+++ b/SWOT_Analysis/SWOT Analysis sample data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I317666\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\MABIRFSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i849308\Documents\GitHub\lumira-extension-viz\SWOT_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Internal environment</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Sequence</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,9 +471,10 @@
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -480,8 +484,11 @@
       <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -491,8 +498,11 @@
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -502,8 +512,11 @@
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -513,8 +526,11 @@
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -524,8 +540,11 @@
       <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -535,8 +554,11 @@
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -546,8 +568,11 @@
       <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -557,8 +582,11 @@
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,8 +596,11 @@
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -579,8 +610,11 @@
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -590,8 +624,11 @@
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -601,8 +638,11 @@
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -612,8 +652,11 @@
       <c r="C13" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -623,8 +666,11 @@
       <c r="C14" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -634,8 +680,11 @@
       <c r="C15" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -645,8 +694,11 @@
       <c r="C16" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -656,8 +708,11 @@
       <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -667,8 +722,11 @@
       <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -678,8 +736,11 @@
       <c r="C19" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -689,8 +750,11 @@
       <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -700,26 +764,29 @@
       <c r="C21" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>